<commit_message>
Backend and frontend for Shop admin
</commit_message>
<xml_diff>
--- a/database-relationship.xlsx
+++ b/database-relationship.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Project\WorldTogether\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5209B54-3E8D-4454-B37D-A4480A83EF76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57A20027-42A9-489F-AA1B-6165D0D8DF4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15255" yWindow="0" windowWidth="10950" windowHeight="11085" xr2:uid="{FF15BF61-1AD8-42DE-9898-09F972EAAF54}"/>
+    <workbookView xWindow="8535" yWindow="105" windowWidth="10950" windowHeight="11085" xr2:uid="{FF15BF61-1AD8-42DE-9898-09F972EAAF54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -650,6 +650,51 @@
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -714,51 +759,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D921007E-89AB-4F4D-ADA5-198EBA7FAFFD}">
   <dimension ref="A1:AE52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E27" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+    <sheetView tabSelected="1" topLeftCell="G4" workbookViewId="0">
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1349,46 +1349,46 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="29"/>
-      <c r="C9" s="29"/>
-      <c r="E9" s="30" t="s">
+      <c r="B9" s="44"/>
+      <c r="C9" s="44"/>
+      <c r="E9" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="I9" s="31" t="s">
+      <c r="F9" s="45"/>
+      <c r="G9" s="45"/>
+      <c r="I9" s="46" t="s">
         <v>35</v>
       </c>
-      <c r="J9" s="31"/>
-      <c r="K9" s="31"/>
-      <c r="M9" s="32" t="s">
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="M9" s="47" t="s">
         <v>38</v>
       </c>
-      <c r="N9" s="32"/>
-      <c r="O9" s="32"/>
-      <c r="Q9" s="27" t="s">
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
+      <c r="Q9" s="42" t="s">
         <v>59</v>
       </c>
-      <c r="R9" s="27"/>
-      <c r="S9" s="27"/>
-      <c r="U9" s="37" t="s">
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="U9" s="52" t="s">
         <v>73</v>
       </c>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
-      <c r="Y9" s="33" t="s">
+      <c r="V9" s="52"/>
+      <c r="W9" s="52"/>
+      <c r="Y9" s="48" t="s">
         <v>77</v>
       </c>
-      <c r="Z9" s="33"/>
-      <c r="AA9" s="33"/>
-      <c r="AC9" s="25" t="s">
+      <c r="Z9" s="48"/>
+      <c r="AA9" s="48"/>
+      <c r="AC9" s="40" t="s">
         <v>97</v>
       </c>
-      <c r="AD9" s="25"/>
-      <c r="AE9" s="25"/>
+      <c r="AD9" s="40"/>
+      <c r="AE9" s="40"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -2197,11 +2197,11 @@
       <c r="O22" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="Q22" s="44" t="s">
+      <c r="Q22" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="R22" s="45"/>
-      <c r="S22" s="46"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="61"/>
       <c r="Y22" s="15" t="s">
         <v>21</v>
       </c>
@@ -2296,11 +2296,11 @@
       <c r="S24" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="U24" s="52" t="s">
+      <c r="U24" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="V24" s="53"/>
-      <c r="W24" s="54"/>
+      <c r="V24" s="31"/>
+      <c r="W24" s="32"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -2383,11 +2383,11 @@
         <v>23</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="I27" s="55" t="s">
+      <c r="I27" s="33" t="s">
         <v>52</v>
       </c>
-      <c r="J27" s="56"/>
-      <c r="K27" s="57"/>
+      <c r="J27" s="34"/>
+      <c r="K27" s="35"/>
       <c r="M27" s="6" t="s">
         <v>48</v>
       </c>
@@ -2415,11 +2415,11 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="28" t="s">
+      <c r="A28" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="B28" s="28"/>
-      <c r="C28" s="28"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
       <c r="E28" s="4" t="s">
         <v>24</v>
       </c>
@@ -2510,11 +2510,11 @@
       <c r="K30" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="M30" s="49" t="s">
+      <c r="M30" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="N30" s="50"/>
-      <c r="O30" s="51"/>
+      <c r="N30" s="28"/>
+      <c r="O30" s="29"/>
       <c r="Q30" s="10" t="s">
         <v>21</v>
       </c>
@@ -2604,11 +2604,11 @@
       <c r="O33" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="Q33" s="34" t="s">
+      <c r="Q33" s="49" t="s">
         <v>72</v>
       </c>
-      <c r="R33" s="35"/>
-      <c r="S33" s="36"/>
+      <c r="R33" s="50"/>
+      <c r="S33" s="51"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="Q34" s="13"/>
@@ -2619,21 +2619,21 @@
       <c r="A35" s="18"/>
       <c r="B35" s="18"/>
       <c r="C35" s="18"/>
-      <c r="E35" s="38" t="s">
+      <c r="E35" s="53" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="39"/>
-      <c r="G35" s="40"/>
-      <c r="I35" s="41" t="s">
+      <c r="F35" s="54"/>
+      <c r="G35" s="55"/>
+      <c r="I35" s="56" t="s">
         <v>54</v>
       </c>
-      <c r="J35" s="42"/>
-      <c r="K35" s="43"/>
-      <c r="M35" s="48" t="s">
+      <c r="J35" s="57"/>
+      <c r="K35" s="58"/>
+      <c r="M35" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="N35" s="48"/>
-      <c r="O35" s="48"/>
+      <c r="N35" s="26"/>
+      <c r="O35" s="26"/>
       <c r="Q35" s="13" t="s">
         <v>69</v>
       </c>
@@ -2643,11 +2643,11 @@
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="26" t="s">
+      <c r="A36" s="41" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="26"/>
-      <c r="C36" s="26"/>
+      <c r="B36" s="41"/>
+      <c r="C36" s="41"/>
       <c r="E36" s="20"/>
       <c r="F36" s="20"/>
       <c r="G36" s="20"/>
@@ -2789,11 +2789,11 @@
         <v>5</v>
       </c>
       <c r="C41" s="22"/>
-      <c r="M41" s="58" t="s">
+      <c r="M41" s="36" t="s">
         <v>118</v>
       </c>
-      <c r="N41" s="58"/>
-      <c r="O41" s="58"/>
+      <c r="N41" s="36"/>
+      <c r="O41" s="36"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
@@ -2803,11 +2803,11 @@
         <v>102</v>
       </c>
       <c r="C42" s="22"/>
-      <c r="I42" s="59" t="s">
+      <c r="I42" s="37" t="s">
         <v>108</v>
       </c>
-      <c r="J42" s="60"/>
-      <c r="K42" s="61"/>
+      <c r="J42" s="38"/>
+      <c r="K42" s="39"/>
       <c r="M42" s="24"/>
       <c r="N42" s="24"/>
       <c r="O42" s="24"/>
@@ -2820,11 +2820,11 @@
         <v>9</v>
       </c>
       <c r="C43" s="22"/>
-      <c r="E43" s="47" t="s">
+      <c r="E43" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="F43" s="47"/>
-      <c r="G43" s="47"/>
+      <c r="F43" s="25"/>
+      <c r="G43" s="25"/>
       <c r="I43" s="19"/>
       <c r="J43" s="19"/>
       <c r="K43" s="19"/>
@@ -2996,13 +2996,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="E43:G43"/>
-    <mergeCell ref="M35:O35"/>
-    <mergeCell ref="M30:O30"/>
-    <mergeCell ref="U24:W24"/>
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="I42:K42"/>
     <mergeCell ref="AC9:AE9"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="Q9:S9"/>
@@ -3017,6 +3010,13 @@
     <mergeCell ref="E35:G35"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="Q22:S22"/>
+    <mergeCell ref="E43:G43"/>
+    <mergeCell ref="M35:O35"/>
+    <mergeCell ref="M30:O30"/>
+    <mergeCell ref="U24:W24"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="I42:K42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Refactor and complete HomeRoute
</commit_message>
<xml_diff>
--- a/database-relationship.xlsx
+++ b/database-relationship.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Resource\Project\WorldTogether\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{989E5033-DBBF-442C-9601-30D5FEDC7AC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEC9ABF5-40AE-4CA6-B68D-3AC0FB7064E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13740" xr2:uid="{FF15BF61-1AD8-42DE-9898-09F972EAAF54}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="125">
   <si>
     <t>Category</t>
   </si>
@@ -397,6 +397,9 @@
   </si>
   <si>
     <t>code</t>
+  </si>
+  <si>
+    <t>quantity</t>
   </si>
 </sst>
 </file>
@@ -634,6 +637,36 @@
     <xf numFmtId="0" fontId="0" fillId="18" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="19" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -710,36 +743,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1070,10 +1073,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D921007E-89AB-4F4D-ADA5-198EBA7FAFFD}">
-  <dimension ref="A1:AE52"/>
+  <dimension ref="A1:AE53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1330,46 +1333,46 @@
       </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="28"/>
-      <c r="C9" s="28"/>
-      <c r="E9" s="29" t="s">
+      <c r="B9" s="38"/>
+      <c r="C9" s="38"/>
+      <c r="E9" s="39" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="29"/>
-      <c r="G9" s="29"/>
-      <c r="I9" s="30" t="s">
+      <c r="F9" s="39"/>
+      <c r="G9" s="39"/>
+      <c r="I9" s="40" t="s">
         <v>34</v>
       </c>
-      <c r="J9" s="30"/>
-      <c r="K9" s="30"/>
-      <c r="M9" s="31" t="s">
+      <c r="J9" s="40"/>
+      <c r="K9" s="40"/>
+      <c r="M9" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="N9" s="31"/>
-      <c r="O9" s="31"/>
-      <c r="Q9" s="26" t="s">
+      <c r="N9" s="41"/>
+      <c r="O9" s="41"/>
+      <c r="Q9" s="36" t="s">
         <v>58</v>
       </c>
-      <c r="R9" s="26"/>
-      <c r="S9" s="26"/>
-      <c r="U9" s="36" t="s">
+      <c r="R9" s="36"/>
+      <c r="S9" s="36"/>
+      <c r="U9" s="46" t="s">
         <v>72</v>
       </c>
-      <c r="V9" s="36"/>
-      <c r="W9" s="36"/>
-      <c r="Y9" s="32" t="s">
+      <c r="V9" s="46"/>
+      <c r="W9" s="46"/>
+      <c r="Y9" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="Z9" s="32"/>
-      <c r="AA9" s="32"/>
-      <c r="AC9" s="24" t="s">
+      <c r="Z9" s="42"/>
+      <c r="AA9" s="42"/>
+      <c r="AC9" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="AD9" s="24"/>
-      <c r="AE9" s="24"/>
+      <c r="AD9" s="34"/>
+      <c r="AE9" s="34"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" s="3"/>
@@ -2178,11 +2181,11 @@
       <c r="O22" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="Q22" s="40" t="s">
+      <c r="Q22" s="50" t="s">
         <v>65</v>
       </c>
-      <c r="R22" s="41"/>
-      <c r="S22" s="42"/>
+      <c r="R22" s="51"/>
+      <c r="S22" s="52"/>
       <c r="Y22" s="15" t="s">
         <v>21</v>
       </c>
@@ -2275,11 +2278,11 @@
       <c r="S24" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="U24" s="47" t="s">
+      <c r="U24" s="57" t="s">
         <v>122</v>
       </c>
-      <c r="V24" s="48"/>
-      <c r="W24" s="49"/>
+      <c r="V24" s="58"/>
+      <c r="W24" s="59"/>
     </row>
     <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
@@ -2362,11 +2365,11 @@
         <v>23</v>
       </c>
       <c r="G27" s="4"/>
-      <c r="I27" s="50" t="s">
+      <c r="I27" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="J27" s="51"/>
-      <c r="K27" s="52"/>
+      <c r="J27" s="25"/>
+      <c r="K27" s="26"/>
       <c r="M27" s="6" t="s">
         <v>47</v>
       </c>
@@ -2394,11 +2397,11 @@
       </c>
     </row>
     <row r="28" spans="1:31" x14ac:dyDescent="0.2">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="37" t="s">
         <v>98</v>
       </c>
-      <c r="B28" s="27"/>
-      <c r="C28" s="27"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
       <c r="E28" s="4" t="s">
         <v>32</v>
       </c>
@@ -2489,11 +2492,11 @@
       <c r="K30" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="M30" s="44" t="s">
+      <c r="M30" s="54" t="s">
         <v>67</v>
       </c>
-      <c r="N30" s="45"/>
-      <c r="O30" s="46"/>
+      <c r="N30" s="55"/>
+      <c r="O30" s="56"/>
       <c r="Q30" s="10" t="s">
         <v>21</v>
       </c>
@@ -2567,11 +2570,11 @@
       <c r="C33" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E33" s="54" t="s">
+      <c r="E33" s="28" t="s">
         <v>106</v>
       </c>
-      <c r="F33" s="55"/>
-      <c r="G33" s="56"/>
+      <c r="F33" s="29"/>
+      <c r="G33" s="30"/>
       <c r="M33" s="11" t="s">
         <v>69</v>
       </c>
@@ -2581,11 +2584,11 @@
       <c r="O33" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="Q33" s="33" t="s">
+      <c r="Q33" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="R33" s="34"/>
-      <c r="S33" s="35"/>
+      <c r="R33" s="44"/>
+      <c r="S33" s="45"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E34" s="20"/>
@@ -2606,16 +2609,16 @@
         <v>23</v>
       </c>
       <c r="G35" s="20"/>
-      <c r="I35" s="37" t="s">
+      <c r="I35" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="J35" s="38"/>
-      <c r="K35" s="39"/>
-      <c r="M35" s="43" t="s">
+      <c r="J35" s="48"/>
+      <c r="K35" s="49"/>
+      <c r="M35" s="53" t="s">
         <v>70</v>
       </c>
-      <c r="N35" s="43"/>
-      <c r="O35" s="43"/>
+      <c r="N35" s="53"/>
+      <c r="O35" s="53"/>
       <c r="Q35" s="13" t="s">
         <v>68</v>
       </c>
@@ -2625,11 +2628,11 @@
       <c r="S35" s="13"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.2">
-      <c r="A36" s="25" t="s">
+      <c r="A36" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="B36" s="25"/>
-      <c r="C36" s="25"/>
+      <c r="B36" s="35"/>
+      <c r="C36" s="35"/>
       <c r="E36" s="20" t="s">
         <v>69</v>
       </c>
@@ -2761,16 +2764,16 @@
         <v>5</v>
       </c>
       <c r="C41" s="22"/>
-      <c r="E41" s="57" t="s">
+      <c r="E41" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="F41" s="58"/>
-      <c r="G41" s="59"/>
-      <c r="M41" s="53" t="s">
+      <c r="F41" s="32"/>
+      <c r="G41" s="33"/>
+      <c r="M41" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="N41" s="53"/>
-      <c r="O41" s="53"/>
+      <c r="N41" s="27"/>
+      <c r="O41" s="27"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A42" s="22" t="s">
@@ -2949,13 +2952,17 @@
       </c>
       <c r="G52" s="19"/>
     </row>
+    <row r="53" spans="5:15" x14ac:dyDescent="0.2">
+      <c r="E53" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="19"/>
+    </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="I27:K27"/>
-    <mergeCell ref="M41:O41"/>
-    <mergeCell ref="E33:G33"/>
-    <mergeCell ref="E41:G41"/>
-    <mergeCell ref="AC9:AE9"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="Q9:S9"/>
     <mergeCell ref="A28:C28"/>
@@ -2963,13 +2970,18 @@
     <mergeCell ref="E9:G9"/>
     <mergeCell ref="I9:K9"/>
     <mergeCell ref="M9:O9"/>
-    <mergeCell ref="Y9:AA9"/>
     <mergeCell ref="Q33:S33"/>
-    <mergeCell ref="U9:W9"/>
     <mergeCell ref="I35:K35"/>
     <mergeCell ref="Q22:S22"/>
     <mergeCell ref="M35:O35"/>
     <mergeCell ref="M30:O30"/>
+    <mergeCell ref="I27:K27"/>
+    <mergeCell ref="M41:O41"/>
+    <mergeCell ref="E33:G33"/>
+    <mergeCell ref="E41:G41"/>
+    <mergeCell ref="AC9:AE9"/>
+    <mergeCell ref="Y9:AA9"/>
+    <mergeCell ref="U9:W9"/>
     <mergeCell ref="U24:W24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>